<commit_message>
fix: update background datatsets and makefile
</commit_message>
<xml_diff>
--- a/references/background_data/a1-a3.xlsx
+++ b/references/background_data/a1-a3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B2D9FF-5BC5-49A3-A305-8E3AD66E4550}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8861C35C-FD2E-4247-981F-5E6D03DECA61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="637">
   <si>
     <t>Name_generic</t>
   </si>
@@ -1927,81 +1927,6 @@
   </si>
   <si>
     <t>Acrylic-based paint for interior applications</t>
-  </si>
-  <si>
-    <t>Paint, enamel, solvent based	kg	"Paint</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> enamel</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> solvent based"	"Solvent-based enamel paint</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> appropriate for use on metals"	0.29		0.0308	0.000423	2.61	0.03		8.20E-13	1.94</t>
-  </si>
-  <si>
-    <t>Tulipwood lumber, 1 inch	kg	"Tulipwood lumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 inch"	"Kiln-dried American Tulipwood (yellow or tulip poplar) hardwood lumber of 1"" nominal thickness as produced in the eastern United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> focusing on the main production technologies and the region-specific characteristics. Tulipwood is frequently used for carvings</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mouldings</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> furniture</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> doors</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> panelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> and cabinets. Link for interactive LCA data tool is provided at the link listed as ""EPD Information""; full LCA report is available at http://naturespackaging.org/wp-content/uploads/2016/02/LifeCycleAssessment-Lumber.pdf."	449	1.6	0.00213	0.000191	0.479	-1.699		2.96E-13	0.0733</t>
-  </si>
-  <si>
-    <t>Stucco, synthetic	kg	"Stucco</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> synthetic"	"Acrylic latex stucco layer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> typically applied over a PVC lath. Base stucco layer with a default thickness of 3/8"" (9.5 mm)."	975	0	0.00529	0.000371	2.51	0.04		5.28E-11	0.137</t>
-  </si>
-  <si>
-    <t>Paint, interior acrylic latex	kg	"Paint</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> interior acrylic latex"	Acrylic-based paint for interior applications	1235	0	0.0091	0.000475	2.4	0.05		1.34E-12	0.173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paint, enamel, solvent based	kg	"Paint	 enamel	" solvent based""	""Solvent-based enamel paint"	" appropriate for use on metals""	0.29		0.0308	0.000423	2.61	0.03		8.20E-13	1.94"									</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tulipwood lumber, 1 inch	kg	"Tulipwood lumber	" 1 inch""	""Kiln-dried American Tulipwood (yellow or tulip poplar) hardwood lumber of 1"""" nominal thickness as produced in the eastern United States"	 focusing on the main production technologies and the region-specific characteristics. Tulipwood is frequently used for carvings	 mouldings	 furniture	 doors	 panelling	" and cabinets. Link for interactive LCA data tool is provided at the link listed as """"EPD Information""""; full LCA report is available at http://naturespackaging.org/wp-content/uploads/2016/02/LifeCycleAssessment-Lumber.pdf.""	449	1.6	0.00213	0.000191	0.479	-1.699		2.96E-13	0.0733"					</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stucco, synthetic	kg	"Stucco	" synthetic""	""Acrylic latex stucco layer"	" typically applied over a PVC lath. Base stucco layer with a default thickness of 3/8"""" (9.5 mm).""	975	0	0.00529	0.000371	2.51	0.04		5.28E-11	0.137"										</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paint, interior acrylic latex	kg	"Paint	" interior acrylic latex""	Acrylic-based paint for interior applications	1235	0	0.0091	0.000475	2.4	0.05		1.34E-12	0.173"											</t>
-  </si>
-  <si>
-    <t xml:space="preserve">283	"Paint	 enamel	" solvent based""	kg	""Paint"	 enamel	" solvent based""	""Solvent-based enamel paint"	" appropriate for use on metals""	0.29		0.0308	0.000423	2.61	0.03		8.2E-13	1.94"																			</t>
-  </si>
-  <si>
-    <t xml:space="preserve">284	"Tulipwood lumber	" 1 inch""	kg	""Tulipwood lumber"	" 1 inch""	""Kiln-dried American Tulipwood (yellow or tulip poplar) hardwood lumber of 1"""" nominal thickness as produced in the eastern United States"	 focusing on the main production technologies and the region-specific characteristics. Tulipwood is frequently used for carvings	 mouldings	 furniture	 doors	 panelling	" and cabinets. Link for interactive LCA data tool is provided at the link listed as """"EPD Information""""; full LCA report is available at http://naturespackaging.org/wp-content/uploads/2016/02/LifeCycleAssessment-Lumber.pdf.""	449	1.6	0.00213	0.000191	0.479	-1.699		2.96E-13	0.0733"																</t>
-  </si>
-  <si>
-    <t xml:space="preserve">285	"Stucco	" synthetic""	kg	""Stucco"	" synthetic""	""Acrylic latex stucco layer"	" typically applied over a PVC lath. Base stucco layer with a default thickness of 3/8"""" (9.5 mm).""	975	0	0.00529	0.000371	2.51	0.04		5.28E-11	0.137"																					</t>
-  </si>
-  <si>
-    <t xml:space="preserve">286	"Paint	" interior acrylic latex""	kg	""Paint"	" interior acrylic latex""	Acrylic-based paint for interior applications	1235	0	0.0091	0.000475	2.4	0.05		1.34E-12	0.173"																						</t>
   </si>
   <si>
     <t>Aluminum storefront system, YKK AP - EPD</t>
@@ -2852,10 +2777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M300"/>
+  <dimension ref="A1:M288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="C292" sqref="C292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,7 +2989,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>661</v>
+        <v>636</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -3254,7 +3179,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>660</v>
+        <v>635</v>
       </c>
       <c r="D11" t="s">
         <v>37</v>
@@ -13544,7 +13469,7 @@
         <v>7.1099999999999997E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>618</v>
       </c>
@@ -13582,7 +13507,7 @@
         <v>0.26806145199999998</v>
       </c>
     </row>
-    <row r="283" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>621</v>
       </c>
@@ -13805,105 +13730,6 @@
       </c>
       <c r="M288">
         <v>0.17299999999999999</v>
-      </c>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>635</v>
-      </c>
-      <c r="B289" t="s">
-        <v>636</v>
-      </c>
-      <c r="C289" t="s">
-        <v>637</v>
-      </c>
-      <c r="D289" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>639</v>
-      </c>
-      <c r="B290" t="s">
-        <v>640</v>
-      </c>
-      <c r="C290" t="s">
-        <v>641</v>
-      </c>
-      <c r="D290" t="s">
-        <v>642</v>
-      </c>
-      <c r="E290" t="s">
-        <v>643</v>
-      </c>
-      <c r="F290" t="s">
-        <v>644</v>
-      </c>
-      <c r="G290" t="s">
-        <v>645</v>
-      </c>
-      <c r="H290" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>647</v>
-      </c>
-      <c r="B291" t="s">
-        <v>648</v>
-      </c>
-      <c r="C291" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>650</v>
-      </c>
-      <c r="B292" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update background datasets
</commit_message>
<xml_diff>
--- a/references/background_data/a1-a3.xlsx
+++ b/references/background_data/a1-a3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8861C35C-FD2E-4247-981F-5E6D03DECA61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1EBAC8-13DA-46D9-AAC6-AB638A3DD37A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2779,8 +2779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="C292" sqref="C292"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,6 +2860,9 @@
       <c r="J2">
         <v>0.04</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
       <c r="L2" s="1">
         <v>5.5799999999999997E-11</v>
       </c>
@@ -2898,6 +2901,9 @@
       <c r="J3">
         <v>0.01</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
       <c r="L3" s="1">
         <v>1.46E-12</v>
       </c>
@@ -2936,6 +2942,9 @@
       <c r="J4">
         <v>0.03</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4">
         <v>3.8500000000000002E-7</v>
       </c>
@@ -2974,6 +2983,9 @@
       <c r="J5">
         <v>0.04</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
       <c r="L5" s="1">
         <v>7.5300000000000002E-13</v>
       </c>
@@ -3012,6 +3024,9 @@
       <c r="J6">
         <v>0</v>
       </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
       <c r="L6" s="1">
         <v>7.9500000000000005E-10</v>
       </c>
@@ -3050,6 +3065,9 @@
       <c r="J7">
         <v>-0.08</v>
       </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
       <c r="L7" s="1">
         <v>8.9000000000000003E-10</v>
       </c>
@@ -3088,6 +3106,9 @@
       <c r="J8">
         <v>-7.0000000000000007E-2</v>
       </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
       <c r="L8" s="1">
         <v>1.1800000000000001E-9</v>
       </c>
@@ -3126,6 +3147,9 @@
       <c r="J9">
         <v>-0.09</v>
       </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
       <c r="L9" s="1">
         <v>6.2300000000000002E-9</v>
       </c>
@@ -3164,6 +3188,9 @@
       <c r="J10">
         <v>-0.08</v>
       </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
       <c r="L10" s="1">
         <v>4.4600000000000002E-8</v>
       </c>
@@ -3202,6 +3229,9 @@
       <c r="J11">
         <v>0</v>
       </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
       <c r="L11" s="1">
         <v>7.9500000000000005E-10</v>
       </c>
@@ -3240,6 +3270,9 @@
       <c r="J12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
       <c r="L12" s="1">
         <v>7.9500000000000005E-10</v>
       </c>
@@ -3278,6 +3311,9 @@
       <c r="J13">
         <v>0</v>
       </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
       <c r="L13" s="1">
         <v>1.05E-10</v>
       </c>
@@ -3316,6 +3352,9 @@
       <c r="J14">
         <v>-0.03</v>
       </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
       <c r="L14" s="1">
         <v>4.9900000000000003E-10</v>
       </c>
@@ -3354,6 +3393,9 @@
       <c r="J15">
         <v>-0.03</v>
       </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
       <c r="L15" s="1">
         <v>4.9900000000000003E-10</v>
       </c>
@@ -3392,6 +3434,9 @@
       <c r="J16">
         <v>-0.57999999999999996</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
       <c r="L16">
         <v>3.0600000000000001E-7</v>
       </c>
@@ -3430,6 +3475,9 @@
       <c r="J17">
         <v>-0.02</v>
       </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
       <c r="L17" s="1">
         <v>7.7600000000000001E-10</v>
       </c>
@@ -3468,6 +3516,9 @@
       <c r="J18">
         <v>-2.1000000000000001E-2</v>
       </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
       <c r="L18" s="1">
         <v>6.3600000000000005E-11</v>
       </c>
@@ -3506,6 +3557,9 @@
       <c r="J19">
         <v>-1.6990000000000001</v>
       </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
       <c r="L19" s="1">
         <v>1.14E-12</v>
       </c>
@@ -3544,6 +3598,9 @@
       <c r="J20">
         <v>-1.4999999999999999E-2</v>
       </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
       <c r="L20" s="1">
         <v>4.0699999999999999E-11</v>
       </c>
@@ -3582,6 +3639,9 @@
       <c r="J21">
         <v>-1.696</v>
       </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
       <c r="L21" s="1">
         <v>1.1099999999999999E-12</v>
       </c>
@@ -3620,6 +3680,9 @@
       <c r="J22">
         <v>-1.698</v>
       </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
       <c r="L22" s="1">
         <v>1.2499999999999999E-12</v>
       </c>
@@ -3658,6 +3721,9 @@
       <c r="J23">
         <v>0</v>
       </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
       <c r="L23" s="1">
         <v>6.8000000000000001E-14</v>
       </c>
@@ -3696,6 +3762,9 @@
       <c r="J24">
         <v>-1.8380000000000001</v>
       </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
       <c r="L24" s="1">
         <v>4.9200000000000002E-13</v>
       </c>
@@ -3734,6 +3803,9 @@
       <c r="J25">
         <v>-1.837</v>
       </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
       <c r="L25" s="1">
         <v>3.8700000000000003E-12</v>
       </c>
@@ -3772,6 +3844,9 @@
       <c r="J26">
         <v>-1.8109999999999999</v>
       </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
       <c r="L26">
         <v>6.1999999999999999E-8</v>
       </c>
@@ -3810,6 +3885,9 @@
       <c r="J27" s="1">
         <v>-3.0000000000000001E-5</v>
       </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
       <c r="L27" s="1">
         <v>3.6300000000000002E-15</v>
       </c>
@@ -3848,6 +3926,9 @@
       <c r="J28">
         <v>-1.76</v>
       </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
       <c r="L28" s="1">
         <v>7.6700000000000002E-9</v>
       </c>
@@ -3886,6 +3967,9 @@
       <c r="J29">
         <v>0</v>
       </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
       <c r="L29" s="1">
         <v>2.6999999999999999E-14</v>
       </c>
@@ -3924,6 +4008,9 @@
       <c r="J30">
         <v>0</v>
       </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
       <c r="L30" s="1">
         <v>2.6999999999999999E-14</v>
       </c>
@@ -3962,6 +4049,9 @@
       <c r="J31">
         <v>-0.01</v>
       </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
       <c r="L31" s="1">
         <v>1.97E-9</v>
       </c>
@@ -4000,6 +4090,9 @@
       <c r="J32">
         <v>0.11</v>
       </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
       <c r="L32" s="1">
         <v>8.9100000000000003E-10</v>
       </c>
@@ -4038,6 +4131,9 @@
       <c r="J33">
         <v>-0.06</v>
       </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
       <c r="L33" s="1">
         <v>6.1900000000000005E-8</v>
       </c>
@@ -4076,6 +4172,9 @@
       <c r="J34">
         <v>-1.83</v>
       </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
       <c r="L34" s="1">
         <v>4.9900000000000003E-12</v>
       </c>
@@ -4114,6 +4213,9 @@
       <c r="J35">
         <v>-1.794</v>
       </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
       <c r="L35" s="1">
         <v>1.56E-10</v>
       </c>
@@ -4152,6 +4254,9 @@
       <c r="J36">
         <v>-1.794</v>
       </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
       <c r="L36" s="1">
         <v>1.56E-10</v>
       </c>
@@ -4190,6 +4295,9 @@
       <c r="J37">
         <v>-0.04</v>
       </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
       <c r="L37" s="1">
         <v>7.8699999999999998E-13</v>
       </c>
@@ -4228,6 +4336,9 @@
       <c r="J38">
         <v>0.4</v>
       </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
       <c r="L38" s="1">
         <v>6.39E-12</v>
       </c>
@@ -4266,6 +4377,9 @@
       <c r="J39">
         <v>0.01</v>
       </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
       <c r="L39" s="1">
         <v>1.34E-10</v>
       </c>
@@ -4304,6 +4418,9 @@
       <c r="J40">
         <v>0</v>
       </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
       <c r="L40" s="1">
         <v>4.7100000000000003E-14</v>
       </c>
@@ -4342,6 +4459,9 @@
       <c r="J41">
         <v>0</v>
       </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
       <c r="L41">
         <v>0</v>
       </c>
@@ -4380,6 +4500,9 @@
       <c r="J42">
         <v>-7.0000000000000007E-2</v>
       </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
       <c r="L42" s="1">
         <v>1.1800000000000001E-9</v>
       </c>
@@ -4418,6 +4541,9 @@
       <c r="J43">
         <v>0</v>
       </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
       <c r="L43" s="1">
         <v>2.41E-12</v>
       </c>
@@ -4456,6 +4582,9 @@
       <c r="J44">
         <v>0.01</v>
       </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
       <c r="L44" s="1">
         <v>1.36E-10</v>
       </c>
@@ -4494,6 +4623,9 @@
       <c r="J45">
         <v>-0.01</v>
       </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
       <c r="L45" s="1">
         <v>-1.6499999999999999E-8</v>
       </c>
@@ -4532,6 +4664,9 @@
       <c r="J46">
         <v>-0.38</v>
       </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
       <c r="L46">
         <v>3.53E-7</v>
       </c>
@@ -4570,6 +4705,9 @@
       <c r="J47">
         <v>-0.193</v>
       </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
       <c r="L47" s="1">
         <v>4.6600000000000003E-13</v>
       </c>
@@ -4608,6 +4746,9 @@
       <c r="J48">
         <v>-0.34</v>
       </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
       <c r="L48">
         <v>1.54E-7</v>
       </c>
@@ -4646,6 +4787,9 @@
       <c r="J49">
         <v>-0.02</v>
       </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
       <c r="L49" s="1">
         <v>1.9399999999999998E-8</v>
       </c>
@@ -4684,6 +4828,9 @@
       <c r="J50">
         <v>-0.01</v>
       </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
       <c r="L50" s="1">
         <v>1.66E-8</v>
       </c>
@@ -4722,6 +4869,9 @@
       <c r="J51">
         <v>0.04</v>
       </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
       <c r="L51" s="1">
         <v>2.2400000000000001E-11</v>
       </c>
@@ -4760,6 +4910,9 @@
       <c r="J52">
         <v>-2E-3</v>
       </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
       <c r="L52" s="1">
         <v>1.6300000000000001E-13</v>
       </c>
@@ -4798,6 +4951,9 @@
       <c r="J53">
         <v>0.01</v>
       </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
       <c r="L53" s="1">
         <v>3.67E-13</v>
       </c>
@@ -4836,6 +4992,9 @@
       <c r="J54">
         <v>-2</v>
       </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
       <c r="L54">
         <v>9.3899999999999999E-6</v>
       </c>
@@ -4874,6 +5033,9 @@
       <c r="J55">
         <v>0</v>
       </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
       <c r="L55" s="1">
         <v>3.3399999999999998E-15</v>
       </c>
@@ -4912,6 +5074,9 @@
       <c r="J56">
         <v>-0.05</v>
       </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
       <c r="L56" s="1">
         <v>5.8199999999999998E-8</v>
       </c>
@@ -4950,6 +5115,9 @@
       <c r="J57">
         <v>-3.0000000000000001E-3</v>
       </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
       <c r="L57" s="1">
         <v>8.4100000000000003E-14</v>
       </c>
@@ -4988,6 +5156,9 @@
       <c r="J58">
         <v>-1.4999999999999999E-2</v>
       </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
       <c r="L58" s="1">
         <v>5.2499999999999999E-9</v>
       </c>
@@ -5026,6 +5197,9 @@
       <c r="J59">
         <v>-0.33</v>
       </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
       <c r="L59">
         <v>2.4299999999999999E-7</v>
       </c>
@@ -5064,6 +5238,9 @@
       <c r="J60">
         <v>0.01</v>
       </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
       <c r="L60" s="1">
         <v>1.1499999999999999E-12</v>
       </c>
@@ -5102,6 +5279,9 @@
       <c r="J61">
         <v>1E-3</v>
       </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
       <c r="L61" s="1">
         <v>6.8099999999999995E-14</v>
       </c>
@@ -5140,6 +5320,9 @@
       <c r="J62">
         <v>0</v>
       </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
       <c r="L62" s="1">
         <v>5.6400000000000002E-13</v>
       </c>
@@ -5178,6 +5361,9 @@
       <c r="J63">
         <v>0</v>
       </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
       <c r="L63" s="1">
         <v>1.1E-12</v>
       </c>
@@ -5216,6 +5402,9 @@
       <c r="J64">
         <v>0</v>
       </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
       <c r="L64" s="1">
         <v>4.7100000000000001E-13</v>
       </c>
@@ -5254,6 +5443,9 @@
       <c r="J65">
         <v>0</v>
       </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
       <c r="L65" s="1">
         <v>7.59E-13</v>
       </c>
@@ -5292,6 +5484,9 @@
       <c r="J66">
         <v>0.01</v>
       </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
       <c r="L66" s="1">
         <v>5.4000000000000002E-13</v>
       </c>
@@ -5330,6 +5525,9 @@
       <c r="J67">
         <v>-1.8109999999999999</v>
       </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
       <c r="L67">
         <v>6.1999999999999999E-8</v>
       </c>
@@ -5368,6 +5566,9 @@
       <c r="J68">
         <v>-1.6970000000000001</v>
       </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
       <c r="L68" s="1">
         <v>1.1E-12</v>
       </c>
@@ -5406,6 +5607,9 @@
       <c r="J69">
         <v>-2.42</v>
       </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
       <c r="L69" s="1">
         <v>4.4300000000000003E-12</v>
       </c>
@@ -5444,6 +5648,9 @@
       <c r="J70">
         <v>-1.5589999999999999</v>
       </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
       <c r="L70" s="1">
         <v>1.1700000000000001E-13</v>
       </c>
@@ -5482,6 +5689,9 @@
       <c r="J71">
         <v>-1.694</v>
       </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
       <c r="L71" s="1">
         <v>7.8699999999999998E-13</v>
       </c>
@@ -5520,6 +5730,9 @@
       <c r="J72">
         <v>0.12</v>
       </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
       <c r="L72" s="1">
         <v>2.0500000000000002E-9</v>
       </c>
@@ -5558,6 +5771,9 @@
       <c r="J73">
         <v>-0.01</v>
       </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
       <c r="L73" s="1">
         <v>2.8699999999999999E-8</v>
       </c>
@@ -5596,6 +5812,9 @@
       <c r="J74">
         <v>-0.02</v>
       </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
       <c r="L74" s="1">
         <v>4.9600000000000001E-8</v>
       </c>
@@ -5634,6 +5853,9 @@
       <c r="J75">
         <v>0.16</v>
       </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
       <c r="L75" s="1">
         <v>2.7800000000000001E-8</v>
       </c>
@@ -5672,6 +5894,9 @@
       <c r="J76">
         <v>-0.01</v>
       </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
       <c r="L76" s="1">
         <v>2.96E-8</v>
       </c>
@@ -5710,6 +5935,9 @@
       <c r="J77">
         <v>-0.02</v>
       </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
       <c r="L77" s="1">
         <v>2.2300000000000001E-8</v>
       </c>
@@ -5748,6 +5976,9 @@
       <c r="J78">
         <v>0.01</v>
       </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
       <c r="L78" s="1">
         <v>2.8999999999999998E-13</v>
       </c>
@@ -5786,6 +6017,9 @@
       <c r="J79">
         <v>-0.10888790700000001</v>
       </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
       <c r="L79" s="1">
         <v>-7.0500000000000003E-9</v>
       </c>
@@ -5824,6 +6058,9 @@
       <c r="J80">
         <v>-1.5920000000000001</v>
       </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
       <c r="L80" s="1">
         <v>4.27E-13</v>
       </c>
@@ -5862,6 +6099,9 @@
       <c r="J81">
         <v>-1.5920000000000001</v>
       </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
       <c r="L81" s="1">
         <v>4.27E-13</v>
       </c>
@@ -5900,6 +6140,9 @@
       <c r="J82">
         <v>-1.732</v>
       </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
       <c r="L82" s="1">
         <v>6.9599999999999997E-10</v>
       </c>
@@ -5938,6 +6181,9 @@
       <c r="J83">
         <v>-1.79</v>
       </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
       <c r="L83" s="1">
         <v>1.6000000000000001E-9</v>
       </c>
@@ -5976,6 +6222,9 @@
       <c r="J84">
         <v>-3.286378E-3</v>
       </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
       <c r="L84" s="1">
         <v>4.9499999999999997E-14</v>
       </c>
@@ -6014,6 +6263,9 @@
       <c r="J85">
         <v>-2.6419989999999999E-3</v>
       </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
       <c r="L85" s="1">
         <v>4.2899999999999999E-14</v>
       </c>
@@ -6052,6 +6304,9 @@
       <c r="J86">
         <v>-1.6278219999999999E-3</v>
       </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
       <c r="L86" s="1">
         <v>3.32E-14</v>
       </c>
@@ -6090,6 +6345,9 @@
       <c r="J87">
         <v>-2.3152849999999998E-3</v>
       </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
       <c r="L87" s="1">
         <v>3.9600000000000003E-14</v>
       </c>
@@ -6128,6 +6386,9 @@
       <c r="J88">
         <v>-2.239595E-3</v>
       </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
       <c r="L88" s="1">
         <v>3.93E-14</v>
       </c>
@@ -6166,6 +6427,9 @@
       <c r="J89">
         <v>-2.0059829999999998E-3</v>
       </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
       <c r="L89" s="1">
         <v>3.6600000000000003E-14</v>
       </c>
@@ -6204,6 +6468,9 @@
       <c r="J90">
         <v>-1.920911E-3</v>
       </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
       <c r="L90" s="1">
         <v>3.6300000000000001E-14</v>
       </c>
@@ -6242,6 +6509,9 @@
       <c r="J91">
         <v>-1.595595E-3</v>
       </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
       <c r="L91" s="1">
         <v>3.32E-14</v>
       </c>
@@ -6280,6 +6550,9 @@
       <c r="J92">
         <v>-2.4194009999999998E-3</v>
       </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
       <c r="L92" s="1">
         <v>4.2099999999999999E-14</v>
       </c>
@@ -6318,6 +6591,9 @@
       <c r="J93">
         <v>-2.3563519999999999E-3</v>
       </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
       <c r="L93" s="1">
         <v>4.23E-14</v>
       </c>
@@ -6356,6 +6632,9 @@
       <c r="J94">
         <v>-2.4328359999999999E-3</v>
       </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
       <c r="L94" s="1">
         <v>4.2099999999999999E-14</v>
       </c>
@@ -6394,6 +6673,9 @@
       <c r="J95">
         <v>-2.399988E-3</v>
       </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
       <c r="L95" s="1">
         <v>4.2099999999999999E-14</v>
       </c>
@@ -6432,6 +6714,9 @@
       <c r="J96">
         <v>-2.509107E-3</v>
       </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
       <c r="L96" s="1">
         <v>4.38E-14</v>
       </c>
@@ -6470,6 +6755,9 @@
       <c r="J97">
         <v>-2.5851300000000002E-3</v>
       </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
       <c r="L97" s="1">
         <v>4.2600000000000003E-14</v>
       </c>
@@ -6508,6 +6796,9 @@
       <c r="J98">
         <v>-2.501409E-3</v>
       </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
       <c r="L98" s="1">
         <v>4.2699999999999997E-14</v>
       </c>
@@ -6546,6 +6837,9 @@
       <c r="J99">
         <v>-2.254593E-3</v>
       </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
       <c r="L99" s="1">
         <v>4.0399999999999997E-14</v>
       </c>
@@ -6584,6 +6878,9 @@
       <c r="J100">
         <v>-2.4028090000000001E-3</v>
       </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
       <c r="L100" s="1">
         <v>4.0900000000000001E-14</v>
       </c>
@@ -6622,6 +6919,9 @@
       <c r="J101">
         <v>-4.1703460000000001E-3</v>
       </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
       <c r="L101" s="1">
         <v>5.7699999999999996E-14</v>
       </c>
@@ -6660,6 +6960,9 @@
       <c r="J102">
         <v>-3.3851609999999998E-3</v>
       </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
       <c r="L102" s="1">
         <v>5.0000000000000002E-14</v>
       </c>
@@ -6698,6 +7001,9 @@
       <c r="J103">
         <v>-2.0872009999999999E-3</v>
       </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
       <c r="L103" s="1">
         <v>3.7499999999999998E-14</v>
       </c>
@@ -6736,6 +7042,9 @@
       <c r="J104">
         <v>-2.96262E-3</v>
       </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
       <c r="L104" s="1">
         <v>4.5699999999999997E-14</v>
       </c>
@@ -6774,6 +7083,9 @@
       <c r="J105">
         <v>-2.890994E-3</v>
       </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
       <c r="L105" s="1">
         <v>4.5500000000000002E-14</v>
       </c>
@@ -6812,6 +7124,9 @@
       <c r="J106">
         <v>-2.564715E-3</v>
       </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
       <c r="L106" s="1">
         <v>4.1800000000000002E-14</v>
       </c>
@@ -6850,6 +7165,9 @@
       <c r="J107">
         <v>-2.4769839999999998E-3</v>
       </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
       <c r="L107" s="1">
         <v>4.15E-14</v>
       </c>
@@ -6888,6 +7206,9 @@
       <c r="J108">
         <v>-2.0367319999999999E-3</v>
       </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
       <c r="L108" s="1">
         <v>3.7300000000000003E-14</v>
       </c>
@@ -6926,6 +7247,9 @@
       <c r="J109">
         <v>-2.9768889999999999E-3</v>
       </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
       <c r="L109" s="1">
         <v>4.7399999999999999E-14</v>
       </c>
@@ -6964,6 +7288,9 @@
       <c r="J110">
         <v>-2.894074E-3</v>
       </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
       <c r="L110" s="1">
         <v>4.75E-14</v>
       </c>
@@ -7002,6 +7329,9 @@
       <c r="J111">
         <v>-2.942301E-3</v>
       </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
       <c r="L111" s="1">
         <v>4.68E-14</v>
       </c>
@@ -7040,6 +7370,9 @@
       <c r="J112">
         <v>-2.9134830000000001E-3</v>
       </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
       <c r="L112" s="1">
         <v>4.7000000000000002E-14</v>
       </c>
@@ -7078,6 +7411,9 @@
       <c r="J113">
         <v>-3.098712E-3</v>
       </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
       <c r="L113" s="1">
         <v>4.9400000000000003E-14</v>
       </c>
@@ -7116,6 +7452,9 @@
       <c r="J114">
         <v>-3.0813680000000001E-3</v>
       </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
       <c r="L114" s="1">
         <v>4.7199999999999997E-14</v>
       </c>
@@ -7154,6 +7493,9 @@
       <c r="J115">
         <v>-3.0246090000000002E-3</v>
       </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
       <c r="L115" s="1">
         <v>4.76E-14</v>
       </c>
@@ -7192,6 +7534,9 @@
       <c r="J116">
         <v>-2.707924E-3</v>
       </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
       <c r="L116" s="1">
         <v>4.4700000000000001E-14</v>
       </c>
@@ -7230,6 +7575,9 @@
       <c r="J117">
         <v>-2.8609249999999998E-3</v>
       </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
       <c r="L117" s="1">
         <v>4.5199999999999999E-14</v>
       </c>
@@ -7268,6 +7616,9 @@
       <c r="J118">
         <v>-4.8838509999999998E-3</v>
       </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
       <c r="L118" s="1">
         <v>6.4799999999999999E-14</v>
       </c>
@@ -7306,6 +7657,9 @@
       <c r="J119">
         <v>-3.9166840000000001E-3</v>
       </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
       <c r="L119" s="1">
         <v>5.5200000000000001E-14</v>
       </c>
@@ -7344,6 +7698,9 @@
       <c r="J120">
         <v>-2.39975E-3</v>
       </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
       <c r="L120" s="1">
         <v>4.0599999999999999E-14</v>
       </c>
@@ -7382,6 +7739,9 @@
       <c r="J121">
         <v>-3.401575E-3</v>
       </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
       <c r="L121" s="1">
         <v>5.0000000000000002E-14</v>
       </c>
@@ -7420,6 +7780,9 @@
       <c r="J122">
         <v>-3.3361089999999999E-3</v>
       </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
       <c r="L122" s="1">
         <v>4.98E-14</v>
       </c>
@@ -7458,6 +7821,9 @@
       <c r="J123">
         <v>-2.9357469999999998E-3</v>
       </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
       <c r="L123" s="1">
         <v>4.5400000000000001E-14</v>
       </c>
@@ -7496,6 +7862,9 @@
       <c r="J124">
         <v>-2.857736E-3</v>
       </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
       <c r="L124" s="1">
         <v>4.53E-14</v>
       </c>
@@ -7534,6 +7903,9 @@
       <c r="J125">
         <v>-2.3439289999999998E-3</v>
       </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
       <c r="L125" s="1">
         <v>4.0300000000000002E-14</v>
       </c>
@@ -7572,6 +7944,9 @@
       <c r="J126">
         <v>-3.545973E-3</v>
       </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
       <c r="L126" s="1">
         <v>5.2699999999999999E-14</v>
       </c>
@@ -7610,6 +7985,9 @@
       <c r="J127">
         <v>-3.4431650000000002E-3</v>
       </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
       <c r="L127" s="1">
         <v>5.2599999999999998E-14</v>
       </c>
@@ -7648,6 +8026,9 @@
       <c r="J128">
         <v>-3.4522390000000002E-3</v>
       </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
       <c r="L128" s="1">
         <v>5.1600000000000002E-14</v>
       </c>
@@ -7686,6 +8067,9 @@
       <c r="J129">
         <v>-3.435844E-3</v>
       </c>
+      <c r="K129">
+        <v>0</v>
+      </c>
       <c r="L129" s="1">
         <v>5.21E-14</v>
       </c>
@@ -7724,6 +8108,9 @@
       <c r="J130">
         <v>-3.7062810000000001E-3</v>
       </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
       <c r="L130" s="1">
         <v>5.4999999999999999E-14</v>
       </c>
@@ -7762,6 +8149,9 @@
       <c r="J131">
         <v>-3.5629780000000001E-3</v>
       </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
       <c r="L131" s="1">
         <v>5.1799999999999998E-14</v>
       </c>
@@ -7800,6 +8190,9 @@
       <c r="J132">
         <v>-3.544228E-3</v>
       </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
       <c r="L132" s="1">
         <v>5.2400000000000003E-14</v>
       </c>
@@ -7838,6 +8231,9 @@
       <c r="J133">
         <v>-3.174138E-3</v>
       </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
       <c r="L133" s="1">
         <v>4.9200000000000001E-14</v>
       </c>
@@ -7876,6 +8272,9 @@
       <c r="J134">
         <v>-3.3053790000000002E-3</v>
       </c>
+      <c r="K134">
+        <v>0</v>
+      </c>
       <c r="L134" s="1">
         <v>4.9200000000000001E-14</v>
       </c>
@@ -7914,6 +8313,9 @@
       <c r="J135">
         <v>0</v>
       </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
       <c r="L135">
         <v>0</v>
       </c>
@@ -7952,6 +8354,9 @@
       <c r="J136">
         <v>2E-3</v>
       </c>
+      <c r="K136">
+        <v>0</v>
+      </c>
       <c r="L136" s="1">
         <v>7.0099999999999999E-14</v>
       </c>
@@ -7990,6 +8395,9 @@
       <c r="J137">
         <v>-1.645</v>
       </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
       <c r="L137" s="1">
         <v>3.9799999999999999E-9</v>
       </c>
@@ -8028,6 +8436,9 @@
       <c r="J138">
         <v>-7.0000000000000007E-2</v>
       </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
       <c r="L138" s="1">
         <v>4.7099999999999998E-8</v>
       </c>
@@ -8066,6 +8477,9 @@
       <c r="J139">
         <v>-0.08</v>
       </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
       <c r="L139" s="1">
         <v>3.8799999999999997E-8</v>
       </c>
@@ -8104,6 +8518,9 @@
       <c r="J140">
         <v>2.9999999999999997E-4</v>
       </c>
+      <c r="K140">
+        <v>0</v>
+      </c>
       <c r="L140" s="1">
         <v>2.0999999999999999E-14</v>
       </c>
@@ -8142,6 +8559,9 @@
       <c r="J141">
         <v>-4.0000000000000001E-3</v>
       </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
       <c r="L141" s="1">
         <v>4.15E-14</v>
       </c>
@@ -8180,6 +8600,9 @@
       <c r="J142">
         <v>0</v>
       </c>
+      <c r="K142">
+        <v>0</v>
+      </c>
       <c r="L142">
         <v>0</v>
       </c>
@@ -8218,6 +8641,9 @@
       <c r="J143">
         <v>-1.732</v>
       </c>
+      <c r="K143">
+        <v>0</v>
+      </c>
       <c r="L143" s="1">
         <v>6.9599999999999997E-10</v>
       </c>
@@ -8256,6 +8682,9 @@
       <c r="J144">
         <v>0.05</v>
       </c>
+      <c r="K144">
+        <v>0</v>
+      </c>
       <c r="L144" s="1">
         <v>1.0700000000000001E-12</v>
       </c>
@@ -8294,6 +8723,9 @@
       <c r="J145">
         <v>0.02</v>
       </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
       <c r="L145" s="1">
         <v>7.1999999999999996E-13</v>
       </c>
@@ -8332,6 +8764,9 @@
       <c r="J146">
         <v>-1.79</v>
       </c>
+      <c r="K146">
+        <v>0</v>
+      </c>
       <c r="L146" s="1">
         <v>1.6000000000000001E-9</v>
       </c>
@@ -8370,6 +8805,9 @@
       <c r="J147">
         <v>0</v>
       </c>
+      <c r="K147">
+        <v>0</v>
+      </c>
       <c r="L147" s="1">
         <v>3.8000000000000002E-14</v>
       </c>
@@ -8408,6 +8846,9 @@
       <c r="J148">
         <v>-0.11</v>
       </c>
+      <c r="K148">
+        <v>0</v>
+      </c>
       <c r="L148">
         <v>1.4000000000000001E-7</v>
       </c>
@@ -8446,6 +8887,9 @@
       <c r="J149">
         <v>-1.794</v>
       </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
       <c r="L149" s="1">
         <v>1.56E-10</v>
       </c>
@@ -8484,6 +8928,9 @@
       <c r="J150">
         <v>-1.794</v>
       </c>
+      <c r="K150">
+        <v>0</v>
+      </c>
       <c r="L150" s="1">
         <v>1.56E-10</v>
       </c>
@@ -8522,6 +8969,9 @@
       <c r="J151">
         <v>0.01</v>
       </c>
+      <c r="K151">
+        <v>0</v>
+      </c>
       <c r="L151" s="1">
         <v>2.98E-10</v>
       </c>
@@ -8560,6 +9010,9 @@
       <c r="J152">
         <v>0.01</v>
       </c>
+      <c r="K152">
+        <v>0</v>
+      </c>
       <c r="L152" s="1">
         <v>7.0100000000000002E-12</v>
       </c>
@@ -8598,6 +9051,9 @@
       <c r="J153">
         <v>-0.02</v>
       </c>
+      <c r="K153">
+        <v>0</v>
+      </c>
       <c r="L153" s="1">
         <v>1.9E-13</v>
       </c>
@@ -8636,6 +9092,9 @@
       <c r="J154">
         <v>0</v>
       </c>
+      <c r="K154">
+        <v>0</v>
+      </c>
       <c r="L154" s="1">
         <v>4.3700000000000002E-12</v>
       </c>
@@ -8674,6 +9133,9 @@
       <c r="J155">
         <v>0.01</v>
       </c>
+      <c r="K155">
+        <v>0</v>
+      </c>
       <c r="L155" s="1">
         <v>1.95E-10</v>
       </c>
@@ -8712,6 +9174,9 @@
       <c r="J156">
         <v>-1.6950000000000001</v>
       </c>
+      <c r="K156">
+        <v>0</v>
+      </c>
       <c r="L156" s="1">
         <v>2.0600000000000001E-12</v>
       </c>
@@ -8750,6 +9215,9 @@
       <c r="J157">
         <v>1E-3</v>
       </c>
+      <c r="K157">
+        <v>0</v>
+      </c>
       <c r="L157" s="1">
         <v>6.34E-14</v>
       </c>
@@ -8788,6 +9256,9 @@
       <c r="J158">
         <v>0</v>
       </c>
+      <c r="K158">
+        <v>0</v>
+      </c>
       <c r="L158" s="1">
         <v>7.2899999999999997E-15</v>
       </c>
@@ -8826,6 +9297,9 @@
       <c r="J159">
         <v>-0.05</v>
       </c>
+      <c r="K159">
+        <v>0</v>
+      </c>
       <c r="L159" s="1">
         <v>1.5400000000000001E-10</v>
       </c>
@@ -8864,6 +9338,9 @@
       <c r="J160">
         <v>-0.03</v>
       </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
       <c r="L160" s="1">
         <v>4.8300000000000002E-12</v>
       </c>
@@ -8902,6 +9379,9 @@
       <c r="J161">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="K161">
+        <v>0</v>
+      </c>
       <c r="L161" s="1">
         <v>1.42E-11</v>
       </c>
@@ -8940,6 +9420,9 @@
       <c r="J162">
         <v>0.01</v>
       </c>
+      <c r="K162">
+        <v>0</v>
+      </c>
       <c r="L162" s="1">
         <v>3.0200000000000003E-11</v>
       </c>
@@ -8978,6 +9461,9 @@
       <c r="J163">
         <v>0.01</v>
       </c>
+      <c r="K163">
+        <v>0</v>
+      </c>
       <c r="L163" s="1">
         <v>1.6300000000000001E-11</v>
       </c>
@@ -9016,6 +9502,9 @@
       <c r="J164">
         <v>-0.04</v>
       </c>
+      <c r="K164">
+        <v>0</v>
+      </c>
       <c r="L164" s="1">
         <v>3.1200000000000001E-8</v>
       </c>
@@ -9054,6 +9543,9 @@
       <c r="J165">
         <v>-0.06</v>
       </c>
+      <c r="K165">
+        <v>0</v>
+      </c>
       <c r="L165">
         <v>5.1E-8</v>
       </c>
@@ -9092,6 +9584,9 @@
       <c r="J166">
         <v>0</v>
       </c>
+      <c r="K166">
+        <v>0</v>
+      </c>
       <c r="L166">
         <v>6.1000000000000004E-8</v>
       </c>
@@ -9130,6 +9625,9 @@
       <c r="J167">
         <v>0</v>
       </c>
+      <c r="K167">
+        <v>0</v>
+      </c>
       <c r="L167" s="1">
         <v>6.13E-8</v>
       </c>
@@ -9168,6 +9666,9 @@
       <c r="J168">
         <v>0</v>
       </c>
+      <c r="K168">
+        <v>0</v>
+      </c>
       <c r="L168" s="1">
         <v>6.3399999999999999E-8</v>
       </c>
@@ -9206,6 +9707,9 @@
       <c r="J169">
         <v>0.01</v>
       </c>
+      <c r="K169">
+        <v>0</v>
+      </c>
       <c r="L169" s="1">
         <v>6.3399999999999999E-8</v>
       </c>
@@ -9244,6 +9748,9 @@
       <c r="J170">
         <v>-0.1</v>
       </c>
+      <c r="K170">
+        <v>0</v>
+      </c>
       <c r="L170" s="1">
         <v>6.7099999999999999E-8</v>
       </c>
@@ -9282,6 +9789,9 @@
       <c r="J171">
         <v>0</v>
       </c>
+      <c r="K171">
+        <v>0</v>
+      </c>
       <c r="L171" s="1">
         <v>6.9300000000000005E-8</v>
       </c>
@@ -9320,6 +9830,9 @@
       <c r="J172">
         <v>-0.05</v>
       </c>
+      <c r="K172">
+        <v>0</v>
+      </c>
       <c r="L172" s="1">
         <v>5.8199999999999998E-8</v>
       </c>
@@ -9358,6 +9871,9 @@
       <c r="J173">
         <v>-0.02</v>
       </c>
+      <c r="K173">
+        <v>0</v>
+      </c>
       <c r="L173" s="1">
         <v>3.1100000000000001E-8</v>
       </c>
@@ -9396,6 +9912,9 @@
       <c r="J174">
         <v>-0.23</v>
       </c>
+      <c r="K174">
+        <v>0</v>
+      </c>
       <c r="L174">
         <v>2.2999999999999999E-7</v>
       </c>
@@ -9434,6 +9953,9 @@
       <c r="J175">
         <v>-0.05</v>
       </c>
+      <c r="K175">
+        <v>0</v>
+      </c>
       <c r="L175" s="1">
         <v>5.8199999999999998E-8</v>
       </c>
@@ -9472,6 +9994,9 @@
       <c r="J176">
         <v>-1E-3</v>
       </c>
+      <c r="K176">
+        <v>0</v>
+      </c>
       <c r="L176" s="1">
         <v>1.7700000000000001E-10</v>
       </c>
@@ -9510,6 +10035,9 @@
       <c r="J177">
         <v>-0.01</v>
       </c>
+      <c r="K177">
+        <v>0</v>
+      </c>
       <c r="L177" s="1">
         <v>4.9099999999999998E-9</v>
       </c>
@@ -9548,6 +10076,9 @@
       <c r="J178">
         <v>-0.01</v>
       </c>
+      <c r="K178">
+        <v>0</v>
+      </c>
       <c r="L178" s="1">
         <v>-8.6100000000000007E-9</v>
       </c>
@@ -9586,6 +10117,9 @@
       <c r="J179">
         <v>-0.01</v>
       </c>
+      <c r="K179">
+        <v>0</v>
+      </c>
       <c r="L179" s="1">
         <v>2.9700000000000001E-8</v>
       </c>
@@ -9624,6 +10158,9 @@
       <c r="J180">
         <v>-0.02</v>
       </c>
+      <c r="K180">
+        <v>0</v>
+      </c>
       <c r="L180" s="1">
         <v>2.29E-8</v>
       </c>
@@ -9662,6 +10199,9 @@
       <c r="J181">
         <v>-0.01</v>
       </c>
+      <c r="K181">
+        <v>0</v>
+      </c>
       <c r="L181" s="1">
         <v>-1.22E-8</v>
       </c>
@@ -9700,6 +10240,9 @@
       <c r="J182">
         <v>0</v>
       </c>
+      <c r="K182">
+        <v>0</v>
+      </c>
       <c r="L182" s="1">
         <v>5.7599999999999997E-13</v>
       </c>
@@ -9738,6 +10281,9 @@
       <c r="J183">
         <v>0</v>
       </c>
+      <c r="K183">
+        <v>0</v>
+      </c>
       <c r="L183" s="1">
         <v>2.1100000000000001E-13</v>
       </c>
@@ -9776,6 +10322,9 @@
       <c r="J184">
         <v>-2.5121309999999999E-3</v>
       </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
       <c r="L184" s="1">
         <v>2.9099999999999997E-14</v>
       </c>
@@ -9814,6 +10363,9 @@
       <c r="J185">
         <v>-2.1340410000000001E-3</v>
       </c>
+      <c r="K185">
+        <v>0</v>
+      </c>
       <c r="L185" s="1">
         <v>2.5599999999999999E-14</v>
       </c>
@@ -9852,6 +10404,9 @@
       <c r="J186">
         <v>-1.3066239999999999E-3</v>
       </c>
+      <c r="K186">
+        <v>0</v>
+      </c>
       <c r="L186" s="1">
         <v>1.7999999999999999E-14</v>
       </c>
@@ -9890,6 +10445,9 @@
       <c r="J187">
         <v>-1.929523E-3</v>
       </c>
+      <c r="K187">
+        <v>0</v>
+      </c>
       <c r="L187" s="1">
         <v>2.3599999999999999E-14</v>
       </c>
@@ -9928,6 +10486,9 @@
       <c r="J188">
         <v>-1.744872E-3</v>
       </c>
+      <c r="K188">
+        <v>0</v>
+      </c>
       <c r="L188" s="1">
         <v>2.1799999999999999E-14</v>
       </c>
@@ -9966,6 +10527,9 @@
       <c r="J189">
         <v>-1.700165E-3</v>
       </c>
+      <c r="K189">
+        <v>0</v>
+      </c>
       <c r="L189" s="1">
         <v>2.1600000000000001E-14</v>
       </c>
@@ -10004,6 +10568,9 @@
       <c r="J190">
         <v>-1.485903E-3</v>
       </c>
+      <c r="K190">
+        <v>0</v>
+      </c>
       <c r="L190" s="1">
         <v>1.96E-14</v>
       </c>
@@ -10042,6 +10609,9 @@
       <c r="J191">
         <v>-1.221654E-3</v>
       </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
       <c r="L191" s="1">
         <v>1.7199999999999999E-14</v>
       </c>
@@ -10080,6 +10650,9 @@
       <c r="J192">
         <v>-1.9539879999999998E-3</v>
       </c>
+      <c r="K192">
+        <v>0</v>
+      </c>
       <c r="L192" s="1">
         <v>2.38E-14</v>
       </c>
@@ -10118,6 +10691,9 @@
       <c r="J193">
         <v>-1.9022010000000001E-3</v>
       </c>
+      <c r="K193">
+        <v>0</v>
+      </c>
       <c r="L193" s="1">
         <v>2.34E-14</v>
       </c>
@@ -10156,6 +10732,9 @@
       <c r="J194">
         <v>-1.9681389999999998E-3</v>
       </c>
+      <c r="K194">
+        <v>0</v>
+      </c>
       <c r="L194" s="1">
         <v>2.41E-14</v>
       </c>
@@ -10194,6 +10773,9 @@
       <c r="J195">
         <v>-1.9672119999999999E-3</v>
       </c>
+      <c r="K195">
+        <v>0</v>
+      </c>
       <c r="L195" s="1">
         <v>2.42E-14</v>
       </c>
@@ -10232,6 +10814,9 @@
       <c r="J196">
         <v>-1.9774049999999998E-3</v>
       </c>
+      <c r="K196">
+        <v>0</v>
+      </c>
       <c r="L196" s="1">
         <v>2.3999999999999999E-14</v>
       </c>
@@ -10270,6 +10855,9 @@
       <c r="J197">
         <v>-2.1327640000000001E-3</v>
       </c>
+      <c r="K197">
+        <v>0</v>
+      </c>
       <c r="L197" s="1">
         <v>2.5899999999999999E-14</v>
       </c>
@@ -10308,6 +10896,9 @@
       <c r="J198">
         <v>-2.0280680000000001E-3</v>
       </c>
+      <c r="K198">
+        <v>0</v>
+      </c>
       <c r="L198" s="1">
         <v>2.4300000000000001E-14</v>
       </c>
@@ -10346,6 +10937,9 @@
       <c r="J199">
         <v>-1.839575E-3</v>
       </c>
+      <c r="K199">
+        <v>0</v>
+      </c>
       <c r="L199" s="1">
         <v>2.2899999999999999E-14</v>
       </c>
@@ -10384,6 +10978,9 @@
       <c r="J200">
         <v>-1.949302E-3</v>
       </c>
+      <c r="K200">
+        <v>0</v>
+      </c>
       <c r="L200" s="1">
         <v>2.3900000000000001E-14</v>
       </c>
@@ -10422,6 +11019,9 @@
       <c r="J201">
         <v>-3.178943E-3</v>
       </c>
+      <c r="K201">
+        <v>0</v>
+      </c>
       <c r="L201" s="1">
         <v>3.5099999999999997E-14</v>
       </c>
@@ -10460,6 +11060,9 @@
       <c r="J202">
         <v>-2.7129810000000002E-3</v>
       </c>
+      <c r="K202">
+        <v>0</v>
+      </c>
       <c r="L202" s="1">
         <v>3.0799999999999999E-14</v>
       </c>
@@ -10498,6 +11101,9 @@
       <c r="J203">
         <v>-1.674914E-3</v>
       </c>
+      <c r="K203">
+        <v>0</v>
+      </c>
       <c r="L203" s="1">
         <v>2.1200000000000001E-14</v>
       </c>
@@ -10536,6 +11142,9 @@
       <c r="J204">
         <v>-2.459588E-3</v>
       </c>
+      <c r="K204">
+        <v>0</v>
+      </c>
       <c r="L204" s="1">
         <v>2.8400000000000001E-14</v>
       </c>
@@ -10574,6 +11183,9 @@
       <c r="J205">
         <v>-2.2160019999999999E-3</v>
       </c>
+      <c r="K205">
+        <v>0</v>
+      </c>
       <c r="L205" s="1">
         <v>2.6E-14</v>
       </c>
@@ -10612,6 +11224,9 @@
       <c r="J206">
         <v>-2.1742770000000001E-3</v>
       </c>
+      <c r="K206">
+        <v>0</v>
+      </c>
       <c r="L206" s="1">
         <v>2.5899999999999999E-14</v>
       </c>
@@ -10650,6 +11265,9 @@
       <c r="J207">
         <v>-1.8861430000000001E-3</v>
       </c>
+      <c r="K207">
+        <v>0</v>
+      </c>
       <c r="L207" s="1">
         <v>2.3100000000000001E-14</v>
       </c>
@@ -10688,6 +11306,9 @@
       <c r="J208">
         <v>-1.563364E-3</v>
       </c>
+      <c r="K208">
+        <v>0</v>
+      </c>
       <c r="L208" s="1">
         <v>2.0100000000000001E-14</v>
       </c>
@@ -10726,6 +11347,9 @@
       <c r="J209">
         <v>-2.397906E-3</v>
       </c>
+      <c r="K209">
+        <v>0</v>
+      </c>
       <c r="L209" s="1">
         <v>2.7799999999999999E-14</v>
       </c>
@@ -10764,6 +11388,9 @@
       <c r="J210">
         <v>-2.337464E-3</v>
       </c>
+      <c r="K210">
+        <v>0</v>
+      </c>
       <c r="L210" s="1">
         <v>2.7399999999999999E-14</v>
       </c>
@@ -10802,6 +11429,9 @@
       <c r="J211">
         <v>-2.3803399999999999E-3</v>
       </c>
+      <c r="K211">
+        <v>0</v>
+      </c>
       <c r="L211" s="1">
         <v>2.7799999999999999E-14</v>
       </c>
@@ -10840,6 +11470,9 @@
       <c r="J212">
         <v>-2.3908520000000002E-3</v>
       </c>
+      <c r="K212">
+        <v>0</v>
+      </c>
       <c r="L212" s="1">
         <v>2.8100000000000001E-14</v>
       </c>
@@ -10878,6 +11511,9 @@
       <c r="J213">
         <v>-2.4278450000000001E-3</v>
       </c>
+      <c r="K213">
+        <v>0</v>
+      </c>
       <c r="L213" s="1">
         <v>2.8100000000000001E-14</v>
       </c>
@@ -10916,6 +11552,9 @@
       <c r="J214">
         <v>-2.5434910000000002E-3</v>
       </c>
+      <c r="K214">
+        <v>0</v>
+      </c>
       <c r="L214" s="1">
         <v>2.9600000000000001E-14</v>
       </c>
@@ -10954,6 +11593,9 @@
       <c r="J215">
         <v>-2.4552020000000001E-3</v>
       </c>
+      <c r="K215">
+        <v>0</v>
+      </c>
       <c r="L215" s="1">
         <v>2.8100000000000001E-14</v>
       </c>
@@ -10992,6 +11634,9 @@
       <c r="J216">
         <v>-2.2304099999999999E-3</v>
       </c>
+      <c r="K216">
+        <v>0</v>
+      </c>
       <c r="L216" s="1">
         <v>2.64E-14</v>
       </c>
@@ -11030,6 +11675,9 @@
       <c r="J217">
         <v>-2.3271400000000001E-3</v>
       </c>
+      <c r="K217">
+        <v>0</v>
+      </c>
       <c r="L217" s="1">
         <v>2.7300000000000001E-14</v>
       </c>
@@ -11068,6 +11716,9 @@
       <c r="J218">
         <v>-3.9411979999999999E-3</v>
       </c>
+      <c r="K218">
+        <v>0</v>
+      </c>
       <c r="L218" s="1">
         <v>4.2199999999999999E-14</v>
       </c>
@@ -11106,6 +11757,9 @@
       <c r="J219">
         <v>-3.3828230000000001E-3</v>
       </c>
+      <c r="K219">
+        <v>0</v>
+      </c>
       <c r="L219" s="1">
         <v>3.7E-14</v>
       </c>
@@ -11144,6 +11798,9 @@
       <c r="J220">
         <v>-2.097036E-3</v>
       </c>
+      <c r="K220">
+        <v>0</v>
+      </c>
       <c r="L220" s="1">
         <v>2.49E-14</v>
       </c>
@@ -11182,6 +11839,9 @@
       <c r="J221">
         <v>-3.0677299999999998E-3</v>
       </c>
+      <c r="K221">
+        <v>0</v>
+      </c>
       <c r="L221" s="1">
         <v>3.4100000000000001E-14</v>
       </c>
@@ -11220,6 +11880,9 @@
       <c r="J222">
         <v>-2.745993E-3</v>
       </c>
+      <c r="K222">
+        <v>0</v>
+      </c>
       <c r="L222" s="1">
         <v>3.1E-14</v>
       </c>
@@ -11258,6 +11921,9 @@
       <c r="J223">
         <v>-2.729184E-3</v>
       </c>
+      <c r="K223">
+        <v>0</v>
+      </c>
       <c r="L223" s="1">
         <v>3.1E-14</v>
       </c>
@@ -11296,6 +11962,9 @@
       <c r="J224">
         <v>-2.3491850000000002E-3</v>
       </c>
+      <c r="K224">
+        <v>0</v>
+      </c>
       <c r="L224" s="1">
         <v>2.7300000000000001E-14</v>
       </c>
@@ -11334,6 +12003,9 @@
       <c r="J225">
         <v>-1.950348E-3</v>
       </c>
+      <c r="K225">
+        <v>0</v>
+      </c>
       <c r="L225" s="1">
         <v>2.3500000000000001E-14</v>
       </c>
@@ -11372,6 +12044,9 @@
       <c r="J226">
         <v>-2.9611419999999999E-3</v>
       </c>
+      <c r="K226">
+        <v>0</v>
+      </c>
       <c r="L226" s="1">
         <v>3.2999999999999998E-14</v>
       </c>
@@ -11410,6 +12085,9 @@
       <c r="J227">
         <v>-2.8745149999999998E-3</v>
       </c>
+      <c r="K227">
+        <v>0</v>
+      </c>
       <c r="L227" s="1">
         <v>3.24E-14</v>
       </c>
@@ -11448,6 +12126,9 @@
       <c r="J228">
         <v>-2.9080270000000001E-3</v>
       </c>
+      <c r="K228">
+        <v>0</v>
+      </c>
       <c r="L228" s="1">
         <v>3.2700000000000002E-14</v>
       </c>
@@ -11486,6 +12167,9 @@
       <c r="J229">
         <v>-2.9273300000000001E-3</v>
       </c>
+      <c r="K229">
+        <v>0</v>
+      </c>
       <c r="L229" s="1">
         <v>3.3099999999999999E-14</v>
       </c>
@@ -11524,6 +12208,9 @@
       <c r="J230">
         <v>-3.0271299999999998E-3</v>
       </c>
+      <c r="K230">
+        <v>0</v>
+      </c>
       <c r="L230" s="1">
         <v>3.3699999999999998E-14</v>
       </c>
@@ -11562,6 +12249,9 @@
       <c r="J231">
         <v>-3.0474949999999999E-3</v>
       </c>
+      <c r="K231">
+        <v>0</v>
+      </c>
       <c r="L231" s="1">
         <v>3.4200000000000002E-14</v>
       </c>
@@ -11600,6 +12290,9 @@
       <c r="J232">
         <v>-2.990042E-3</v>
       </c>
+      <c r="K232">
+        <v>0</v>
+      </c>
       <c r="L232" s="1">
         <v>3.3099999999999999E-14</v>
       </c>
@@ -11638,6 +12331,9 @@
       <c r="J233">
         <v>-2.68104E-3</v>
       </c>
+      <c r="K233">
+        <v>0</v>
+      </c>
       <c r="L233" s="1">
         <v>3.0599999999999997E-14</v>
       </c>
@@ -11676,6 +12372,9 @@
       <c r="J234">
         <v>-2.8027719999999998E-3</v>
       </c>
+      <c r="K234">
+        <v>0</v>
+      </c>
       <c r="L234" s="1">
         <v>3.17E-14</v>
       </c>
@@ -11714,6 +12413,9 @@
       <c r="J235">
         <v>-4.0541919999999999E-3</v>
       </c>
+      <c r="K235">
+        <v>0</v>
+      </c>
       <c r="L235" s="1">
         <v>4.3200000000000001E-14</v>
       </c>
@@ -11752,6 +12454,9 @@
       <c r="J236">
         <v>-3.4806759999999998E-3</v>
       </c>
+      <c r="K236">
+        <v>0</v>
+      </c>
       <c r="L236" s="1">
         <v>3.7900000000000001E-14</v>
       </c>
@@ -11790,6 +12495,9 @@
       <c r="J237">
         <v>-2.1581199999999999E-3</v>
       </c>
+      <c r="K237">
+        <v>0</v>
+      </c>
       <c r="L237" s="1">
         <v>2.5599999999999999E-14</v>
       </c>
@@ -11828,6 +12536,9 @@
       <c r="J238">
         <v>-3.162125E-3</v>
       </c>
+      <c r="K238">
+        <v>0</v>
+      </c>
       <c r="L238" s="1">
         <v>3.5000000000000002E-14</v>
       </c>
@@ -11866,6 +12577,9 @@
       <c r="J239">
         <v>-2.82993E-3</v>
       </c>
+      <c r="K239">
+        <v>0</v>
+      </c>
       <c r="L239" s="1">
         <v>3.1800000000000001E-14</v>
       </c>
@@ -11904,6 +12618,9 @@
       <c r="J240">
         <v>-2.8152199999999998E-3</v>
       </c>
+      <c r="K240">
+        <v>0</v>
+      </c>
       <c r="L240" s="1">
         <v>3.1800000000000001E-14</v>
       </c>
@@ -11942,6 +12659,9 @@
       <c r="J241">
         <v>-2.4188539999999998E-3</v>
       </c>
+      <c r="K241">
+        <v>0</v>
+      </c>
       <c r="L241" s="1">
         <v>2.8000000000000001E-14</v>
       </c>
@@ -11980,6 +12700,9 @@
       <c r="J242">
         <v>-2.0067890000000001E-3</v>
       </c>
+      <c r="K242">
+        <v>0</v>
+      </c>
       <c r="L242" s="1">
         <v>2.41E-14</v>
       </c>
@@ -12018,6 +12741,9 @@
       <c r="J243">
         <v>-3.007844E-3</v>
       </c>
+      <c r="K243">
+        <v>0</v>
+      </c>
       <c r="L243" s="1">
         <v>3.3599999999999997E-14</v>
       </c>
@@ -12056,6 +12782,9 @@
       <c r="J244">
         <v>-2.923602E-3</v>
       </c>
+      <c r="K244">
+        <v>0</v>
+      </c>
       <c r="L244" s="1">
         <v>3.2999999999999998E-14</v>
       </c>
@@ -12094,6 +12823,9 @@
       <c r="J245">
         <v>-2.9524500000000001E-3</v>
       </c>
+      <c r="K245">
+        <v>0</v>
+      </c>
       <c r="L245" s="1">
         <v>3.3300000000000001E-14</v>
       </c>
@@ -12132,6 +12864,9 @@
       <c r="J246">
         <v>-2.9558129999999998E-3</v>
       </c>
+      <c r="K246">
+        <v>0</v>
+      </c>
       <c r="L246" s="1">
         <v>3.3599999999999997E-14</v>
       </c>
@@ -12170,6 +12905,9 @@
       <c r="J247">
         <v>-3.069193E-3</v>
       </c>
+      <c r="K247">
+        <v>0</v>
+      </c>
       <c r="L247" s="1">
         <v>3.4300000000000003E-14</v>
       </c>
@@ -12208,6 +12946,9 @@
       <c r="J248">
         <v>-3.1046379999999998E-3</v>
       </c>
+      <c r="K248">
+        <v>0</v>
+      </c>
       <c r="L248" s="1">
         <v>3.4900000000000001E-14</v>
       </c>
@@ -12246,6 +12987,9 @@
       <c r="J249">
         <v>-3.0446340000000001E-3</v>
       </c>
+      <c r="K249">
+        <v>0</v>
+      </c>
       <c r="L249" s="1">
         <v>3.3699999999999998E-14</v>
       </c>
@@ -12284,6 +13028,9 @@
       <c r="J250">
         <v>-2.7320270000000002E-3</v>
       </c>
+      <c r="K250">
+        <v>0</v>
+      </c>
       <c r="L250" s="1">
         <v>3.1200000000000002E-14</v>
       </c>
@@ -12322,6 +13069,9 @@
       <c r="J251">
         <v>-2.8561379999999998E-3</v>
       </c>
+      <c r="K251">
+        <v>0</v>
+      </c>
       <c r="L251" s="1">
         <v>3.24E-14</v>
       </c>
@@ -12360,6 +13110,9 @@
       <c r="J252">
         <v>-4.7491529999999999E-3</v>
       </c>
+      <c r="K252">
+        <v>0</v>
+      </c>
       <c r="L252" s="1">
         <v>4.9599999999999998E-14</v>
       </c>
@@ -12398,6 +13151,9 @@
       <c r="J253">
         <v>-4.0975760000000003E-3</v>
       </c>
+      <c r="K253">
+        <v>0</v>
+      </c>
       <c r="L253" s="1">
         <v>4.3599999999999998E-14</v>
       </c>
@@ -12436,6 +13192,9 @@
       <c r="J254">
         <v>-2.5512130000000001E-3</v>
       </c>
+      <c r="K254">
+        <v>0</v>
+      </c>
       <c r="L254" s="1">
         <v>2.9000000000000003E-14</v>
       </c>
@@ -12474,6 +13233,9 @@
       <c r="J255">
         <v>-3.7308799999999998E-3</v>
       </c>
+      <c r="K255">
+        <v>0</v>
+      </c>
       <c r="L255" s="1">
         <v>4.0200000000000002E-14</v>
       </c>
@@ -12512,6 +13274,9 @@
       <c r="J256">
         <v>-3.320974E-3</v>
       </c>
+      <c r="K256">
+        <v>0</v>
+      </c>
       <c r="L256" s="1">
         <v>3.6300000000000001E-14</v>
       </c>
@@ -12550,6 +13315,9 @@
       <c r="J257">
         <v>-3.3345850000000002E-3</v>
       </c>
+      <c r="K257">
+        <v>0</v>
+      </c>
       <c r="L257" s="1">
         <v>3.6400000000000001E-14</v>
       </c>
@@ -12588,6 +13356,9 @@
       <c r="J258">
         <v>-2.842851E-3</v>
       </c>
+      <c r="K258">
+        <v>0</v>
+      </c>
       <c r="L258" s="1">
         <v>3.17E-14</v>
       </c>
@@ -12626,6 +13397,9 @@
       <c r="J259">
         <v>-2.3626540000000001E-3</v>
       </c>
+      <c r="K259">
+        <v>0</v>
+      </c>
       <c r="L259" s="1">
         <v>2.72E-14</v>
       </c>
@@ -12664,6 +13438,9 @@
       <c r="J260">
         <v>-3.6212380000000001E-3</v>
       </c>
+      <c r="K260">
+        <v>0</v>
+      </c>
       <c r="L260" s="1">
         <v>3.92E-14</v>
       </c>
@@ -12702,6 +13479,9 @@
       <c r="J261">
         <v>-3.502191E-3</v>
       </c>
+      <c r="K261">
+        <v>0</v>
+      </c>
       <c r="L261" s="1">
         <v>3.8299999999999998E-14</v>
       </c>
@@ -12740,6 +13520,9 @@
       <c r="J262">
         <v>-3.4821000000000001E-3</v>
       </c>
+      <c r="K262">
+        <v>0</v>
+      </c>
       <c r="L262" s="1">
         <v>3.8100000000000003E-14</v>
       </c>
@@ -12778,6 +13561,9 @@
       <c r="J263">
         <v>-3.4960080000000001E-3</v>
       </c>
+      <c r="K263">
+        <v>0</v>
+      </c>
       <c r="L263" s="1">
         <v>3.8600000000000001E-14</v>
       </c>
@@ -12816,6 +13602,9 @@
       <c r="J264">
         <v>-3.7243509999999999E-3</v>
       </c>
+      <c r="K264">
+        <v>0</v>
+      </c>
       <c r="L264" s="1">
         <v>4.0399999999999997E-14</v>
       </c>
@@ -12854,6 +13643,9 @@
       <c r="J265">
         <v>-3.6083700000000001E-3</v>
       </c>
+      <c r="K265">
+        <v>0</v>
+      </c>
       <c r="L265" s="1">
         <v>3.9500000000000002E-14</v>
       </c>
@@ -12892,6 +13684,9 @@
       <c r="J266">
         <v>-3.582689E-3</v>
       </c>
+      <c r="K266">
+        <v>0</v>
+      </c>
       <c r="L266" s="1">
         <v>3.8600000000000001E-14</v>
       </c>
@@ -12930,6 +13725,9 @@
       <c r="J267">
         <v>-3.2234540000000002E-3</v>
       </c>
+      <c r="K267">
+        <v>0</v>
+      </c>
       <c r="L267" s="1">
         <v>3.5700000000000002E-14</v>
       </c>
@@ -12968,6 +13766,9 @@
       <c r="J268">
         <v>-3.3161750000000002E-3</v>
       </c>
+      <c r="K268">
+        <v>0</v>
+      </c>
       <c r="L268" s="1">
         <v>3.6500000000000002E-14</v>
       </c>
@@ -13006,6 +13807,9 @@
       <c r="J269">
         <v>-0.02</v>
       </c>
+      <c r="K269">
+        <v>0</v>
+      </c>
       <c r="L269" s="1">
         <v>9.949999999999999E-13</v>
       </c>
@@ -13044,6 +13848,9 @@
       <c r="J270">
         <v>0.01</v>
       </c>
+      <c r="K270">
+        <v>0</v>
+      </c>
       <c r="L270" s="1">
         <v>1.8899999999999999E-10</v>
       </c>
@@ -13082,6 +13889,9 @@
       <c r="J271">
         <v>6.0000000000000001E-3</v>
       </c>
+      <c r="K271">
+        <v>0</v>
+      </c>
       <c r="L271" s="1">
         <v>4.3599999999999998E-14</v>
       </c>
@@ -13120,6 +13930,9 @@
       <c r="J272">
         <v>7.0000000000000001E-3</v>
       </c>
+      <c r="K272">
+        <v>0</v>
+      </c>
       <c r="L272" s="1">
         <v>4.8500000000000002E-14</v>
       </c>
@@ -13158,6 +13971,9 @@
       <c r="J273">
         <v>0</v>
       </c>
+      <c r="K273">
+        <v>0</v>
+      </c>
       <c r="L273" s="1">
         <v>2.64E-14</v>
       </c>
@@ -13196,6 +14012,9 @@
       <c r="J274">
         <v>-1.696</v>
       </c>
+      <c r="K274">
+        <v>0</v>
+      </c>
       <c r="L274" s="1">
         <v>1.3399999999999999E-12</v>
       </c>
@@ -13234,6 +14053,9 @@
       <c r="J275">
         <v>2.14E-4</v>
       </c>
+      <c r="K275">
+        <v>0</v>
+      </c>
       <c r="L275" s="1">
         <v>2.3800000000000002E-16</v>
       </c>
@@ -13272,6 +14094,9 @@
       <c r="J276">
         <v>-1.7050000000000001</v>
       </c>
+      <c r="K276">
+        <v>0</v>
+      </c>
       <c r="L276" s="1">
         <v>2.0499999999999999E-12</v>
       </c>
@@ -13310,6 +14135,9 @@
       <c r="J277">
         <v>0.11</v>
       </c>
+      <c r="K277">
+        <v>0</v>
+      </c>
       <c r="L277" s="1">
         <v>8.9100000000000003E-10</v>
       </c>
@@ -13348,6 +14176,9 @@
       <c r="J278">
         <v>0.1</v>
       </c>
+      <c r="K278">
+        <v>0</v>
+      </c>
       <c r="L278" s="1">
         <v>8.9100000000000003E-10</v>
       </c>
@@ -13386,6 +14217,9 @@
       <c r="J279">
         <v>-0.01</v>
       </c>
+      <c r="K279">
+        <v>0</v>
+      </c>
       <c r="L279" s="1">
         <v>7.5199999999999996E-11</v>
       </c>
@@ -13424,6 +14258,9 @@
       <c r="J280">
         <v>-1.83</v>
       </c>
+      <c r="K280">
+        <v>0</v>
+      </c>
       <c r="L280" s="1">
         <v>4.9900000000000003E-12</v>
       </c>
@@ -13462,6 +14299,9 @@
       <c r="J281">
         <v>0.01</v>
       </c>
+      <c r="K281">
+        <v>0</v>
+      </c>
       <c r="L281" s="1">
         <v>1.7999999999999999E-11</v>
       </c>
@@ -13500,6 +14340,9 @@
       <c r="J282">
         <v>0</v>
       </c>
+      <c r="K282">
+        <v>0</v>
+      </c>
       <c r="L282">
         <v>3.2499999999999997E-5</v>
       </c>
@@ -13538,6 +14381,9 @@
       <c r="J283">
         <v>0</v>
       </c>
+      <c r="K283">
+        <v>0</v>
+      </c>
       <c r="L283">
         <v>4.3099999999999997E-5</v>
       </c>
@@ -13576,6 +14422,9 @@
       <c r="J284">
         <v>0.2</v>
       </c>
+      <c r="K284">
+        <v>0</v>
+      </c>
       <c r="L284" s="1">
         <v>-6.6399999999999998E-11</v>
       </c>
@@ -13611,6 +14460,9 @@
       <c r="J285">
         <v>0.03</v>
       </c>
+      <c r="K285">
+        <v>0</v>
+      </c>
       <c r="L285" s="1">
         <v>8.2000000000000004E-13</v>
       </c>
@@ -13649,6 +14501,9 @@
       <c r="J286">
         <v>-1.6990000000000001</v>
       </c>
+      <c r="K286">
+        <v>0</v>
+      </c>
       <c r="L286" s="1">
         <v>2.96E-13</v>
       </c>
@@ -13687,6 +14542,9 @@
       <c r="J287">
         <v>0.04</v>
       </c>
+      <c r="K287">
+        <v>0</v>
+      </c>
       <c r="L287" s="1">
         <v>5.2800000000000001E-11</v>
       </c>
@@ -13724,6 +14582,9 @@
       </c>
       <c r="J288">
         <v>0.05</v>
+      </c>
+      <c r="K288">
+        <v>0</v>
       </c>
       <c r="L288" s="1">
         <v>1.3399999999999999E-12</v>

</xml_diff>

<commit_message>
feat: add stored carbon to prebuilt scenarios
</commit_message>
<xml_diff>
--- a/references/background_data/a1-a3.xlsx
+++ b/references/background_data/a1-a3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A7B2AA-7806-4278-A3A2-B09EAE6A4F70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226999FD-9A06-4A7A-BA63-BC692B693B47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2779,8 +2779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M288"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="F286" sqref="F286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14448,6 +14448,9 @@
       <c r="E285">
         <v>0.28999999999999998</v>
       </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
       <c r="G285">
         <v>3.0800000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
fix: update to bom, background datasets
</commit_message>
<xml_diff>
--- a/references/background_data/a1-a3.xlsx
+++ b/references/background_data/a1-a3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226999FD-9A06-4A7A-BA63-BC692B693B47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76393A6-216A-477E-B80D-FCA05FD542FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="640">
   <si>
     <t>Name_generic</t>
   </si>
@@ -1933,6 +1933,15 @@
   </si>
   <si>
     <t>stored_carbon_mfg</t>
+  </si>
+  <si>
+    <t>Light wood framing, SPF</t>
+  </si>
+  <si>
+    <t>Domestic softwood, US, AWC - EPD</t>
+  </si>
+  <si>
+    <t>Kiln-dried and planed softwood dimensional lumber for standard framing or planking. Industry-wide EPD from the American Wood Council.</t>
   </si>
 </sst>
 </file>
@@ -2777,14 +2786,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M288"/>
+  <dimension ref="A1:M289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="F286" sqref="F286"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="M289" sqref="A289:M289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="135.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14596,7 +14606,49 @@
         <v>0.17299999999999999</v>
       </c>
     </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>637</v>
+      </c>
+      <c r="B289" t="s">
+        <v>13</v>
+      </c>
+      <c r="C289" t="s">
+        <v>638</v>
+      </c>
+      <c r="D289" t="s">
+        <v>639</v>
+      </c>
+      <c r="E289">
+        <v>433.57</v>
+      </c>
+      <c r="F289">
+        <v>1.44</v>
+      </c>
+      <c r="G289">
+        <v>1.8500000000000001E-3</v>
+      </c>
+      <c r="H289" s="1">
+        <v>7.5599999999999994E-5</v>
+      </c>
+      <c r="I289">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="J289">
+        <v>-1.8380000000000001</v>
+      </c>
+      <c r="K289">
+        <v>0</v>
+      </c>
+      <c r="L289" s="1">
+        <v>7.9799999999999995E-12</v>
+      </c>
+      <c r="M289">
+        <v>3.1899999999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>